<commit_message>
Repaired sheets naming error
</commit_message>
<xml_diff>
--- a/Daily Reports/Coffee Shop 1.xlsx
+++ b/Daily Reports/Coffee Shop 1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin.grigorescu\Documents\UiPath\ExcelConsolidation\Daily Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\UiPath\UiPathAcademy Excel reports consolication\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9292BC7C-C458-4C82-A205-D63EFED33463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>

</xml_diff>